<commit_message>
Moved a function definition to the spreadsheet
</commit_message>
<xml_diff>
--- a/services/core/DNP3Agent/data/mesa_functions.xlsx
+++ b/services/core/DNP3Agent/data/mesa_functions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43660" yWindow="-7560" windowWidth="21920" windowHeight="15400" tabRatio="500" firstSheet="18" activeTab="25"/>
+    <workbookView xWindow="56280" yWindow="-7100" windowWidth="21920" windowHeight="15400" tabRatio="500" firstSheet="19" activeTab="26"/>
   </bookViews>
   <sheets>
     <sheet name="disconnect" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,7 @@
     <sheet name="schedule_creation" sheetId="24" r:id="rId24"/>
     <sheet name="schedule_enable" sheetId="25" r:id="rId25"/>
     <sheet name="curve" sheetId="26" r:id="rId26"/>
+    <sheet name="schedule" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="434">
   <si>
     <t xml:space="preserve">Step </t>
   </si>
@@ -1345,6 +1346,15 @@
   </si>
   <si>
     <t>CurveStart</t>
+  </si>
+  <si>
+    <t>Schedule Edit Selector</t>
+  </si>
+  <si>
+    <t>Schedule Start</t>
+  </si>
+  <si>
+    <t>Schedule Enable</t>
   </si>
 </sst>
 </file>
@@ -1424,7 +1434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1494,6 +1504,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5841,8 +5855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6022,6 +6036,87 @@
       <c r="D14" s="13" t="s">
         <v>406</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="13"/>
+    <col min="2" max="2" width="21.33203125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>431</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>432</v>
+      </c>
+      <c r="C3" s="24"/>
+      <c r="D3" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>